<commit_message>
Update database demo and README
</commit_message>
<xml_diff>
--- a/Demo.xlsx
+++ b/Demo.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC83670B-7EAD-44C2-B226-10B5CE699BC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251B30D9-508C-4ABE-AE76-2E16C4AED893}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="2120" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2115" yWindow="2115" windowWidth="14400" windowHeight="7365" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="用户" sheetId="1" r:id="rId1"/>
-    <sheet name="词典" sheetId="2" r:id="rId2"/>
-    <sheet name="单词本" sheetId="3" r:id="rId3"/>
-    <sheet name="收录" sheetId="4" r:id="rId4"/>
-    <sheet name="单词计划" sheetId="5" r:id="rId5"/>
-    <sheet name="统计信息" sheetId="6" r:id="rId6"/>
+    <sheet name="USER" sheetId="1" r:id="rId1"/>
+    <sheet name="DICTIONARY" sheetId="2" r:id="rId2"/>
+    <sheet name="VOCABULARY" sheetId="3" r:id="rId3"/>
+    <sheet name="TAKES" sheetId="4" r:id="rId4"/>
+    <sheet name="PLAN" sheetId="5" r:id="rId5"/>
+    <sheet name="RECORD" sheetId="6" r:id="rId6"/>
+    <sheet name="FEEDBACK" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,32 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="96">
   <si>
     <t>UID</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>用户名</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>手机</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>性别</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>学历</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>年级</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>char(32)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -79,10 +60,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>大学</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>0002</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -95,10 +72,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>高中</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>0003</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -111,18 +84,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>单词</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>音标</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>释义</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -132,10 +93,6 @@
   </si>
   <si>
     <t>hello</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>哈喽</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -189,10 +146,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>世界</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>[w</t>
     </r>
@@ -249,27 +202,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>蟒蛇</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>VID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>名称</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>单词数量</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>建议用时</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>类别</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -336,10 +269,6 @@
       </rPr>
       <t>sti]</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>匆忙的</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -397,103 +326,243 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>消失</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>TID</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>SID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0006</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>char(64)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>123456</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LM@123.com</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WM@123.com</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LW@123.com</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>char(128)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"10 0 0 0"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uname</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PW</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mail</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sex</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grade</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>English</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chinese</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Psymbol</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>n. 巨蟒</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>adj. 轻率的；匆忙的
+n. (Hasty)人名；(英)黑斯蒂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>int. 喂；哈罗
+n. 表示问候， 惊奇或唤起注意时的用语</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>n. 世界；领域；世俗；全人类；物质生活</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>vi. 消失；突然不见；成为零
+vt. 使不见，使消失
+n. 弱化音</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Psymbol(phonetic symbol)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>仅供参考，设计数据库时请选择合适的数据类型</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要考虑如何把不同的意思、词性分开</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Education</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>男/女/未知</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vname</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Proficiency</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Score</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ahour</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ahour(Active hour)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要考虑如何保存一天的活跃时间</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>熟练度</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>SID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>时间</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>背单词数量</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>小测成绩</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>活跃时间</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>0006</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>密码</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>char(64)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>123456</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>邮箱</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LM@123.com</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>WM@123.com</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LW@123.com</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>词性</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>char(8)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>n</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>adj</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>熟练度</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>char(128)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"10 0 0 0"</t>
+    <t>Pnumber</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avatar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>//base64</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Null</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Undergraduate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Senior</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Primary Junior Senior Undergraduate Graduate Doctor Others</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要有个默认初始头像，0/null，仅供参考</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>想到再添</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>暂时只用0，1，2，3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>比如：onehot形式？</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Info</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-12-13</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-12-10</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OMG! I'v never seen such perfect APP!</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Why didn't I find such great software earlier!!!</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>大部分反馈应该是中文的</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -504,7 +573,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,8 +613,23 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -554,12 +638,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -576,8 +665,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -585,8 +689,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
@@ -599,12 +706,19 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="3" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="3" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="标题 1" xfId="1" builtinId="16"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="解释性文本" xfId="2" builtinId="53"/>
+    <cellStyle name="注释" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -882,148 +996,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="3"/>
-    <col min="3" max="3" width="8.6640625" style="3"/>
-    <col min="4" max="4" width="13.25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" style="3"/>
+    <col min="4" max="4" width="9" style="3"/>
+    <col min="5" max="5" width="13.25" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="3">
+        <v>13900008888</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="3">
+        <v>18900006666</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="3">
+        <v>13800007777</v>
+      </c>
+      <c r="G5" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="H5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="3">
-        <v>13900008888</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="3">
-        <v>18900006666</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="3">
-        <v>13800007777</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
+      <c r="H6" s="14" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1035,142 +1180,129 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D376C4C6-4333-413F-9126-222A87DC383F}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="3"/>
+    <col min="3" max="3" width="20.125" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="29.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D6" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1182,100 +1314,106 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DBA8FB-88F1-4EB0-BD92-66203B0D2E84}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="2" max="2" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="6.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="14" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1289,89 +1427,89 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1382,107 +1520,116 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1E3B8C-363E-4281-8021-AA5C49CCC953}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>23</v>
@@ -1496,72 +1643,76 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16DA4D9-ADF8-4DDE-AE7A-567244F2D7C8}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="9" style="3"/>
-    <col min="3" max="3" width="11.58203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.75" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="9">
         <v>43800</v>
@@ -1573,18 +1724,18 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C4" s="9">
         <v>43800</v>
@@ -1596,18 +1747,18 @@
         <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="G4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C5" s="9">
         <v>43800</v>
@@ -1619,18 +1770,18 @@
         <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="G5">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" s="9">
         <v>43801</v>
@@ -1642,18 +1793,18 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="G6">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C7" s="9">
         <v>43801</v>
@@ -1665,18 +1816,18 @@
         <v>75</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="G7">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C8" s="9">
         <v>43801</v>
@@ -1688,11 +1839,113 @@
         <v>74</v>
       </c>
       <c r="F8" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="G8">
         <v>22</v>
       </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G10" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F12B2EC6-5F84-45C3-B09F-CDDF01645688}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J11:J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>